<commit_message>
fixed dornbirn email adress
</commit_message>
<xml_diff>
--- a/gemeinden_XLSX.xlsx
+++ b/gemeinden_XLSX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelhuber/Desktop/projects/gemeinde_scraper/github/oe_gemeinden/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14BD1C9-9BD0-1646-90D8-6F610F93EF52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B84C8FF-4D46-DD49-B521-25C92774327E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12220" windowWidth="19200" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="12220" windowWidth="19200" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18691,9 +18691,6 @@
     <t>gemeinde@wolfurt.at</t>
   </si>
   <si>
-    <t>stadt_@dornbirn.at</t>
-  </si>
-  <si>
     <t>stadt@hohenems.at</t>
   </si>
   <si>
@@ -18824,6 +18821,9 @@
   </si>
   <si>
     <t>buergermeisterin.kahr@stadt.graz.at</t>
+  </si>
+  <si>
+    <t>stadt@dornbirn.at</t>
   </si>
 </sst>
 </file>
@@ -19262,8 +19262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2095"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1424" zoomScale="90" workbookViewId="0">
-      <selection activeCell="E1435" sqref="E1435"/>
+    <sheetView tabSelected="1" topLeftCell="A1882" zoomScale="90" workbookViewId="0">
+      <selection activeCell="E2069" sqref="E2069"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19279,13 +19279,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6263</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>6264</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6265</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6266</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -28632,7 +28632,7 @@
         <v>3622</v>
       </c>
       <c r="D551" s="2" t="s">
-        <v>6252</v>
+        <v>6251</v>
       </c>
       <c r="E551" t="s">
         <v>4401</v>
@@ -33409,10 +33409,10 @@
         <v>2851</v>
       </c>
       <c r="D832" s="2" t="s">
+        <v>6255</v>
+      </c>
+      <c r="E832" t="s">
         <v>6256</v>
-      </c>
-      <c r="E832" t="s">
-        <v>6257</v>
       </c>
     </row>
     <row r="833" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -34984,7 +34984,7 @@
         <v>40445</v>
       </c>
       <c r="B925" s="5" t="s">
-        <v>6253</v>
+        <v>6252</v>
       </c>
       <c r="C925" s="3">
         <v>5122</v>
@@ -43663,7 +43663,7 @@
         <v>3514</v>
       </c>
       <c r="E1435" t="s">
-        <v>6267</v>
+        <v>6266</v>
       </c>
     </row>
     <row r="1436" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -44249,7 +44249,7 @@
         <v>60651</v>
       </c>
       <c r="B1470" s="5" t="s">
-        <v>6254</v>
+        <v>6253</v>
       </c>
       <c r="C1470" s="3">
         <v>8124</v>
@@ -45694,7 +45694,7 @@
         <v>61262</v>
       </c>
       <c r="B1555" s="5" t="s">
-        <v>6255</v>
+        <v>6254</v>
       </c>
       <c r="C1555" s="3">
         <v>8960</v>
@@ -50919,10 +50919,10 @@
         <v>6528</v>
       </c>
       <c r="D1862" s="2" t="s">
+        <v>6261</v>
+      </c>
+      <c r="E1862" t="s">
         <v>6262</v>
-      </c>
-      <c r="E1862" t="s">
-        <v>6263</v>
       </c>
     </row>
     <row r="1863" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -52194,10 +52194,10 @@
         <v>6611</v>
       </c>
       <c r="D1937" s="2" t="s">
+        <v>6259</v>
+      </c>
+      <c r="E1937" t="s">
         <v>6260</v>
-      </c>
-      <c r="E1937" t="s">
-        <v>6261</v>
       </c>
     </row>
     <row r="1938" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54098,7 +54098,7 @@
         <v>6942</v>
       </c>
       <c r="D2049" s="2" t="s">
-        <v>6258</v>
+        <v>6257</v>
       </c>
       <c r="E2049" t="s">
         <v>4993</v>
@@ -54404,7 +54404,7 @@
         <v>6934</v>
       </c>
       <c r="D2067" s="2" t="s">
-        <v>6259</v>
+        <v>6258</v>
       </c>
       <c r="E2067" t="s">
         <v>6217</v>
@@ -54441,7 +54441,7 @@
         <v>4144</v>
       </c>
       <c r="E2069" t="s">
-        <v>6223</v>
+        <v>6267</v>
       </c>
     </row>
     <row r="2070" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54458,7 +54458,7 @@
         <v>4145</v>
       </c>
       <c r="E2070" t="s">
-        <v>6224</v>
+        <v>6223</v>
       </c>
     </row>
     <row r="2071" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54475,7 +54475,7 @@
         <v>4146</v>
       </c>
       <c r="E2071" t="s">
-        <v>6225</v>
+        <v>6224</v>
       </c>
     </row>
     <row r="2072" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54492,7 +54492,7 @@
         <v>4147</v>
       </c>
       <c r="E2072" t="s">
-        <v>6226</v>
+        <v>6225</v>
       </c>
     </row>
     <row r="2073" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54509,7 +54509,7 @@
         <v>4148</v>
       </c>
       <c r="E2073" t="s">
-        <v>6227</v>
+        <v>6226</v>
       </c>
     </row>
     <row r="2074" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54526,7 +54526,7 @@
         <v>4149</v>
       </c>
       <c r="E2074" t="s">
-        <v>6228</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="2075" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54543,7 +54543,7 @@
         <v>4150</v>
       </c>
       <c r="E2075" t="s">
-        <v>6229</v>
+        <v>6228</v>
       </c>
     </row>
     <row r="2076" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54560,7 +54560,7 @@
         <v>4151</v>
       </c>
       <c r="E2076" t="s">
-        <v>6230</v>
+        <v>6229</v>
       </c>
     </row>
     <row r="2077" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54577,7 +54577,7 @@
         <v>4152</v>
       </c>
       <c r="E2077" t="s">
-        <v>6231</v>
+        <v>6230</v>
       </c>
     </row>
     <row r="2078" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54594,7 +54594,7 @@
         <v>4153</v>
       </c>
       <c r="E2078" t="s">
-        <v>6232</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="2079" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54611,7 +54611,7 @@
         <v>4154</v>
       </c>
       <c r="E2079" t="s">
-        <v>6233</v>
+        <v>6232</v>
       </c>
     </row>
     <row r="2080" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54628,7 +54628,7 @@
         <v>4155</v>
       </c>
       <c r="E2080" t="s">
-        <v>6234</v>
+        <v>6233</v>
       </c>
     </row>
     <row r="2081" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54645,7 +54645,7 @@
         <v>4156</v>
       </c>
       <c r="E2081" t="s">
-        <v>6235</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="2082" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54662,7 +54662,7 @@
         <v>4157</v>
       </c>
       <c r="E2082" t="s">
-        <v>6236</v>
+        <v>6235</v>
       </c>
     </row>
     <row r="2083" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54679,7 +54679,7 @@
         <v>4158</v>
       </c>
       <c r="E2083" t="s">
-        <v>6237</v>
+        <v>6236</v>
       </c>
     </row>
     <row r="2084" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54696,7 +54696,7 @@
         <v>4159</v>
       </c>
       <c r="E2084" t="s">
-        <v>6238</v>
+        <v>6237</v>
       </c>
     </row>
     <row r="2085" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54713,7 +54713,7 @@
         <v>4160</v>
       </c>
       <c r="E2085" t="s">
-        <v>6239</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="2086" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54730,7 +54730,7 @@
         <v>4161</v>
       </c>
       <c r="E2086" t="s">
-        <v>6240</v>
+        <v>6239</v>
       </c>
     </row>
     <row r="2087" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54747,7 +54747,7 @@
         <v>4162</v>
       </c>
       <c r="E2087" t="s">
-        <v>6241</v>
+        <v>6240</v>
       </c>
     </row>
     <row r="2088" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54764,7 +54764,7 @@
         <v>4163</v>
       </c>
       <c r="E2088" t="s">
-        <v>6242</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="2089" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54781,7 +54781,7 @@
         <v>4164</v>
       </c>
       <c r="E2089" t="s">
-        <v>6243</v>
+        <v>6242</v>
       </c>
     </row>
     <row r="2090" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54798,7 +54798,7 @@
         <v>4165</v>
       </c>
       <c r="E2090" t="s">
-        <v>6244</v>
+        <v>6243</v>
       </c>
     </row>
     <row r="2091" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54815,7 +54815,7 @@
         <v>4166</v>
       </c>
       <c r="E2091" t="s">
-        <v>6245</v>
+        <v>6244</v>
       </c>
     </row>
     <row r="2092" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54823,16 +54823,16 @@
         <v>80421</v>
       </c>
       <c r="B2092" s="5" t="s">
-        <v>6250</v>
+        <v>6249</v>
       </c>
       <c r="C2092" s="3">
         <v>6832</v>
       </c>
       <c r="D2092" s="2" t="s">
-        <v>6251</v>
+        <v>6250</v>
       </c>
       <c r="E2092" t="s">
-        <v>6246</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="2093" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54849,7 +54849,7 @@
         <v>4167</v>
       </c>
       <c r="E2093" t="s">
-        <v>6247</v>
+        <v>6246</v>
       </c>
     </row>
     <row r="2094" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54866,7 +54866,7 @@
         <v>4168</v>
       </c>
       <c r="E2094" t="s">
-        <v>6248</v>
+        <v>6247</v>
       </c>
     </row>
     <row r="2095" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -54883,7 +54883,7 @@
         <v>4169</v>
       </c>
       <c r="E2095" t="s">
-        <v>6249</v>
+        <v>6248</v>
       </c>
     </row>
   </sheetData>
@@ -56978,6 +56978,7 @@
     <hyperlink ref="D2" r:id="rId2087" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D1862" r:id="rId2088" xr:uid="{4F6A1E72-82F5-3547-8FD6-397C8C9B131F}"/>
     <hyperlink ref="E1435" r:id="rId2089" xr:uid="{50EB4A6C-1119-2443-A10A-CCBEAC0D5643}"/>
+    <hyperlink ref="E2069" r:id="rId2090" xr:uid="{265332BF-8A2A-BA44-98F6-22007AEE8F46}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>